<commit_message>
Finally got trees working
</commit_message>
<xml_diff>
--- a/24-25Year/Fall24/DES214/walkingsim2/3DWalkingSimulator.xlsx
+++ b/24-25Year/Fall24/DES214/walkingsim2/3DWalkingSimulator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaos\Documents\DIT Work\DITRepo\24-25Year\Fall24\DES214\walkingsim2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KingLoui1221\Documents\DIT Stuff\DITRepo\DITWork\24-25Year\Fall24\DES214\walkingsim2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1D5522-4C7D-4985-8092-344289921D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07B1CED-50CF-40C4-8604-D8AFDC38F92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -2468,18 +2468,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="6.54296875" style="30" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="130.54296875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="9.08984375" style="2"/>
+    <col min="1" max="1" width="6.5703125" style="30" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="130.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="23" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" ht="24" thickBot="1">
@@ -2495,7 +2495,7 @@
       </c>
       <c r="E1" s="22"/>
     </row>
-    <row r="2" spans="1:5" ht="47" thickBot="1">
+    <row r="2" spans="1:5" ht="48" thickBot="1">
       <c r="A2" s="45"/>
       <c r="B2" s="44" t="s">
         <v>29</v>
@@ -2504,7 +2504,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="4" customHeight="1">
+    <row r="3" spans="1:5" ht="3.95" customHeight="1">
       <c r="A3" s="54"/>
       <c r="B3" s="57" t="s">
         <v>30</v>
@@ -2518,12 +2518,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="8.15" customHeight="1" thickBot="1">
+    <row r="5" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="A5" s="56"/>
       <c r="B5" s="59"/>
       <c r="C5" s="27"/>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" ht="19" thickBot="1">
+    <row r="6" spans="1:5" s="3" customFormat="1" ht="38.25" thickBot="1">
       <c r="A6" s="37">
         <f>IF(LEFT(B6,2)="No",0,IF(LEFT(B6,7)="Partial",0.02,IF(LEFT(B6,4)="Full",0.04,"n/a")))</f>
         <v>0</v>
@@ -2536,7 +2536,7 @@
       </c>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="7" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A7" s="37">
         <f>IF(LEFT(B7,2)="No",-0.1,IF(LEFT(B7,7)="Partial",0,IF(LEFT(B7,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="E7" s="25"/>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="8" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A8" s="38">
         <f>IF(LEFT(B8,2)="No",-0.1,IF(LEFT(B8,7)="Partial",0,IF(LEFT(B8,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2562,7 +2562,7 @@
       </c>
       <c r="E8" s="25"/>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="9" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A9" s="38">
         <f>IF(LEFT(B9,2)="No",-0.1,IF(LEFT(B9,7)="Partial",0,IF(LEFT(B9,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="10" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A10" s="38">
         <f>IF(LEFT(B10,2)="No",-0.1,IF(LEFT(B10,7)="Partial",0,IF(LEFT(B10,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="E10" s="25"/>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" ht="31.5" thickBot="1">
+    <row r="11" spans="1:5" s="3" customFormat="1" ht="32.25" thickBot="1">
       <c r="A11" s="39">
         <f>IF(LEFT(B11,2)="No",-0.1,IF(LEFT(B11,7)="Partial",0,IF(LEFT(B11,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="E11" s="25"/>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="12" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A12" s="38" t="str">
         <f>IF(LEFT(B12,2)="No",0,IF(LEFT(B12,7)="Partial",0.01,IF(LEFT(B12,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="13" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A13" s="38" t="str">
         <f>IF(LEFT(B13,2)="No",0,IF(LEFT(B13,7)="Partial",0.01,IF(LEFT(B13,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2623,7 +2623,7 @@
       </c>
       <c r="E13" s="25"/>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="14" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A14" s="38" t="str">
         <f>IF(LEFT(B14,2)="No",0,IF(LEFT(B14,7)="Partial",0.01,IF(LEFT(B14,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2634,7 +2634,7 @@
       </c>
       <c r="E14" s="25"/>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="15" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A15" s="39" t="str">
         <f>IF(LEFT(B15,2)="No",0,IF(LEFT(B15,7)="Partial",0.01,IF(LEFT(B15,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2645,10 +2645,10 @@
       </c>
       <c r="E15" s="25"/>
     </row>
-    <row r="16" spans="1:5" ht="8.15" customHeight="1" thickBot="1">
+    <row r="16" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C16" s="27"/>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="17" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A17" s="36">
         <f>IF(LEFT(B17,2)="No",0,IF(LEFT(B17,7)="Partial",0.02,IF(LEFT(B17,4)="Full",0.04,"n/a")))</f>
         <v>0</v>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="E17" s="25"/>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="18" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A18" s="38">
         <f>IF(LEFT(B18,2)="No",-0.1,IF(LEFT(B18,7)="Partial",0,IF(LEFT(B18,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2674,7 +2674,7 @@
       </c>
       <c r="E18" s="25"/>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1">
+    <row r="19" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A19" s="38">
         <f>IF(LEFT(B19,2)="No",-0.1,IF(LEFT(B19,7)="Partial",0,IF(LEFT(B19,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="21" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A21" s="38">
         <f>IF(LEFT(B21,2)="No",-0.1,IF(LEFT(B21,7)="Partial",0,IF(LEFT(B21,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="22" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A22" s="38">
         <f>IF(LEFT(B22,2)="No",-0.1,IF(LEFT(B22,7)="Partial",0,IF(LEFT(B22,4)="Full",0.02,"n/a")))</f>
         <v>0.02</v>
@@ -2726,7 +2726,7 @@
       </c>
       <c r="E22" s="25"/>
     </row>
-    <row r="23" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="23" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A23" s="37" t="str">
         <f>IF(LEFT(B23,2)="No",0,IF(LEFT(B23,7)="Partial",0.01,IF(LEFT(B23,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="E23" s="25"/>
     </row>
-    <row r="24" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="24" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A24" s="38" t="str">
         <f>IF(LEFT(B24,2)="No",0,IF(LEFT(B24,7)="Partial",0.01,IF(LEFT(B24,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2748,7 +2748,7 @@
       </c>
       <c r="E24" s="25"/>
     </row>
-    <row r="25" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="25" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A25" s="38" t="str">
         <f>IF(LEFT(B25,2)="No",0,IF(LEFT(B25,7)="Partial",0.01,IF(LEFT(B25,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="E25" s="25"/>
     </row>
-    <row r="26" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="26" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A26" s="39" t="str">
         <f>IF(LEFT(B26,2)="No",0,IF(LEFT(B26,7)="Partial",0.01,IF(LEFT(B26,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2770,10 +2770,10 @@
       </c>
       <c r="E26" s="25"/>
     </row>
-    <row r="27" spans="1:5" ht="8.15" customHeight="1" thickBot="1">
+    <row r="27" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C27" s="27"/>
     </row>
-    <row r="28" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="28" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A28" s="36">
         <f>IF(LEFT(B28,2)="No",0,IF(LEFT(B28,7)="Partial",0.02,IF(LEFT(B28,4)="Full",0.04,"n/a")))</f>
         <v>0</v>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="E28" s="25"/>
     </row>
-    <row r="29" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="29" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A29" s="37">
         <f>IF(LEFT(B29,2)="No",-0.1,IF(LEFT(B29,7)="Partial",0,IF(LEFT(B29,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2799,7 +2799,7 @@
       </c>
       <c r="E29" s="25"/>
     </row>
-    <row r="30" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="30" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A30" s="38">
         <f>IF(LEFT(B30,2)="No",-0.1,IF(LEFT(B30,7)="Partial",0,IF(LEFT(B30,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2812,7 +2812,7 @@
       </c>
       <c r="E30" s="24"/>
     </row>
-    <row r="31" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="31" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A31" s="38">
         <f>IF(LEFT(B31,2)="No",-0.1,IF(LEFT(B31,7)="Partial",0,IF(LEFT(B31,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2825,7 +2825,7 @@
       </c>
       <c r="E31" s="24"/>
     </row>
-    <row r="32" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="32" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A32" s="38">
         <f>IF(LEFT(B32,2)="No",-0.1,IF(LEFT(B32,7)="Partial",0,IF(LEFT(B32,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="E32" s="24"/>
     </row>
-    <row r="33" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="33" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A33" s="39">
         <f>IF(LEFT(B33,2)="No",-0.1,IF(LEFT(B33,7)="Partial",0,IF(LEFT(B33,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2851,7 +2851,7 @@
       </c>
       <c r="E33" s="25"/>
     </row>
-    <row r="34" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="34" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A34" s="38" t="str">
         <f>IF(LEFT(B34,2)="No",0,IF(LEFT(B34,7)="Partial",0.01,IF(LEFT(B34,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="E34" s="25"/>
     </row>
-    <row r="35" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="35" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A35" s="38" t="str">
         <f>IF(LEFT(B35,2)="No",0,IF(LEFT(B35,7)="Partial",0.01,IF(LEFT(B35,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2873,7 +2873,7 @@
       </c>
       <c r="E35" s="25"/>
     </row>
-    <row r="36" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="36" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A36" s="38" t="str">
         <f>IF(LEFT(B36,2)="No",0,IF(LEFT(B36,7)="Partial",0.01,IF(LEFT(B36,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2884,7 +2884,7 @@
       </c>
       <c r="E36" s="25"/>
     </row>
-    <row r="37" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="37" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A37" s="39" t="str">
         <f>IF(LEFT(B37,2)="No",0,IF(LEFT(B37,7)="Partial",0.01,IF(LEFT(B37,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2895,10 +2895,10 @@
       </c>
       <c r="E37" s="25"/>
     </row>
-    <row r="38" spans="1:5" ht="8.15" customHeight="1" thickBot="1">
+    <row r="38" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C38" s="27"/>
     </row>
-    <row r="39" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="39" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A39" s="36">
         <f>IF(LEFT(B39,2)="No",0,IF(LEFT(B39,7)="Partial",0.02,IF(LEFT(B39,4)="Full",0.04,"n/a")))</f>
         <v>0</v>
@@ -2911,7 +2911,7 @@
       </c>
       <c r="E39" s="24"/>
     </row>
-    <row r="40" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="40" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A40" s="37">
         <f>IF(LEFT(B40,2)="No",-0.1,IF(LEFT(B40,7)="Partial",0,IF(LEFT(B40,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2924,7 +2924,7 @@
       </c>
       <c r="E40" s="25"/>
     </row>
-    <row r="41" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="41" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A41" s="38">
         <f>IF(LEFT(B41,2)="No",-0.1,IF(LEFT(B41,7)="Partial",0,IF(LEFT(B41,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="E41" s="24"/>
     </row>
-    <row r="42" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="42" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A42" s="38">
         <f>IF(LEFT(B42,2)="No",-0.1,IF(LEFT(B42,7)="Partial",0,IF(LEFT(B42,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2950,7 +2950,7 @@
       </c>
       <c r="E42" s="24"/>
     </row>
-    <row r="43" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="43" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A43" s="38">
         <f>IF(LEFT(B43,2)="No",-0.1,IF(LEFT(B43,7)="Partial",0,IF(LEFT(B43,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2963,7 +2963,7 @@
       </c>
       <c r="E43" s="24"/>
     </row>
-    <row r="44" spans="1:5" s="3" customFormat="1" ht="31.5" thickBot="1">
+    <row r="44" spans="1:5" s="3" customFormat="1" ht="32.25" thickBot="1">
       <c r="A44" s="39">
         <f>IF(LEFT(B44,2)="No",-0.1,IF(LEFT(B44,7)="Partial",0,IF(LEFT(B44,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -2976,7 +2976,7 @@
       </c>
       <c r="E44" s="25"/>
     </row>
-    <row r="45" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="45" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A45" s="37" t="str">
         <f>IF(LEFT(B45,2)="No",0,IF(LEFT(B45,7)="Partial",0.01,IF(LEFT(B45,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="E45" s="25"/>
     </row>
-    <row r="46" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="46" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A46" s="38" t="str">
         <f>IF(LEFT(B46,2)="No",0,IF(LEFT(B46,7)="Partial",0.01,IF(LEFT(B46,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -2998,7 +2998,7 @@
       </c>
       <c r="E46" s="25"/>
     </row>
-    <row r="47" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="47" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A47" s="38" t="str">
         <f>IF(LEFT(B47,2)="No",0,IF(LEFT(B47,7)="Partial",0.01,IF(LEFT(B47,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="E47" s="25"/>
     </row>
-    <row r="48" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="48" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A48" s="39" t="str">
         <f>IF(LEFT(B48,2)="No",0,IF(LEFT(B48,7)="Partial",0.01,IF(LEFT(B48,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3020,10 +3020,10 @@
       </c>
       <c r="E48" s="25"/>
     </row>
-    <row r="49" spans="1:5" ht="8.15" customHeight="1" thickBot="1">
+    <row r="49" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="C49" s="27"/>
     </row>
-    <row r="50" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="50" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A50" s="36">
         <f>IF(LEFT(B50,2)="No",0,IF(LEFT(B50,7)="Partial",0.02,IF(LEFT(B50,4)="Full",0.04,"n/a")))</f>
         <v>0</v>
@@ -3036,7 +3036,7 @@
       </c>
       <c r="E50" s="25"/>
     </row>
-    <row r="51" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="51" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A51" s="37">
         <f>IF(LEFT(B51,2)="No",-0.1,IF(LEFT(B51,7)="Partial",0,IF(LEFT(B51,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3049,7 +3049,7 @@
       </c>
       <c r="E51" s="25"/>
     </row>
-    <row r="52" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="52" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A52" s="38">
         <f>IF(LEFT(B52,2)="No",-0.1,IF(LEFT(B52,7)="Partial",0,IF(LEFT(B52,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3062,7 +3062,7 @@
       </c>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="53" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A53" s="38">
         <f>IF(LEFT(B53,2)="No",-0.1,IF(LEFT(B53,7)="Partial",0,IF(LEFT(B53,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3075,7 +3075,7 @@
       </c>
       <c r="E53" s="24"/>
     </row>
-    <row r="54" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="54" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A54" s="38">
         <f>IF(LEFT(B54,2)="No",-0.1,IF(LEFT(B54,7)="Partial",0,IF(LEFT(B54,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="E54" s="24"/>
     </row>
-    <row r="55" spans="1:5" s="3" customFormat="1" ht="31.5" thickBot="1">
+    <row r="55" spans="1:5" s="3" customFormat="1" ht="32.25" thickBot="1">
       <c r="A55" s="39">
         <f>IF(LEFT(B55,2)="No",-0.1,IF(LEFT(B55,7)="Partial",0,IF(LEFT(B55,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="E55" s="25"/>
     </row>
-    <row r="56" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="56" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A56" s="38" t="str">
         <f>IF(LEFT(B56,2)="No",0,IF(LEFT(B56,7)="Partial",0.01,IF(LEFT(B56,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="E56" s="25"/>
     </row>
-    <row r="57" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="57" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A57" s="38" t="str">
         <f>IF(LEFT(B57,2)="No",0,IF(LEFT(B57,7)="Partial",0.01,IF(LEFT(B57,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="E57" s="25"/>
     </row>
-    <row r="58" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="58" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A58" s="38" t="str">
         <f>IF(LEFT(B58,2)="No",0,IF(LEFT(B58,7)="Partial",0.01,IF(LEFT(B58,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="E58" s="25"/>
     </row>
-    <row r="59" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="59" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A59" s="39" t="str">
         <f>IF(LEFT(B59,2)="No",0,IF(LEFT(B59,7)="Partial",0.01,IF(LEFT(B59,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3145,10 +3145,10 @@
       </c>
       <c r="E59" s="25"/>
     </row>
-    <row r="60" spans="1:5" ht="8" customHeight="1" thickBot="1">
+    <row r="60" spans="1:5" ht="8.1" customHeight="1" thickBot="1">
       <c r="E60" s="25"/>
     </row>
-    <row r="61" spans="1:5" s="50" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="61" spans="1:5" s="50" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A61" s="48">
         <f>IF(LEFT(B61,1)="5",0.05,IF(LEFT(B61,1)="4",0.04,IF(LEFT(B61,1)="3",0.03,IF(LEFT(B61,1)="2",0.02,IF(LEFT(B61,1)="1",0.01,IF(LEFT(B61,1)="O",0,IF(LEFT(B61,1)="L",0,"n/a")))))))</f>
         <v>0</v>
@@ -3161,7 +3161,7 @@
       </c>
       <c r="E61" s="51"/>
     </row>
-    <row r="62" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="62" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A62" s="37">
         <f>IF(LEFT(B62,2)="No",-0.1,IF(LEFT(B62,7)="Partial",0,IF(LEFT(B62,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3174,7 +3174,7 @@
       </c>
       <c r="E62" s="25"/>
     </row>
-    <row r="63" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="63" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A63" s="38">
         <f>IF(LEFT(B63,2)="No",-0.1,IF(LEFT(B63,7)="Partial",0,IF(LEFT(B63,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3187,7 +3187,7 @@
       </c>
       <c r="E63" s="25"/>
     </row>
-    <row r="64" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="64" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A64" s="38">
         <f>IF(LEFT(B64,2)="No",-0.1,IF(LEFT(B64,7)="Partial",0,IF(LEFT(B64,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3200,7 +3200,7 @@
       </c>
       <c r="E64" s="26"/>
     </row>
-    <row r="65" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="65" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A65" s="38">
         <f>IF(LEFT(B65,2)="No",-0.1,IF(LEFT(B65,7)="Partial",0,IF(LEFT(B65,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="E65" s="26"/>
     </row>
-    <row r="66" spans="1:5" ht="16" customHeight="1" thickBot="1">
+    <row r="66" spans="1:5" ht="15.95" customHeight="1" thickBot="1">
       <c r="A66" s="39">
         <f>IF(LEFT(B66,2)="No",-0.1,IF(LEFT(B66,7)="Partial",0,IF(LEFT(B66,4)="Full",0.02,"n/a")))</f>
         <v>-0.1</v>
@@ -3226,7 +3226,7 @@
       </c>
       <c r="E66" s="25"/>
     </row>
-    <row r="67" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="67" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A67" s="37" t="str">
         <f>IF(LEFT(B67,2)="No",0,IF(LEFT(B67,7)="Partial",0.01,IF(LEFT(B67,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3237,7 +3237,7 @@
       </c>
       <c r="E67" s="25"/>
     </row>
-    <row r="68" spans="1:5" s="3" customFormat="1" ht="31">
+    <row r="68" spans="1:5" s="3" customFormat="1" ht="31.5">
       <c r="A68" s="38" t="str">
         <f>IF(LEFT(B68,2)="No",0,IF(LEFT(B68,7)="Partial",0.01,IF(LEFT(B68,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3248,7 +3248,7 @@
       </c>
       <c r="E68" s="25"/>
     </row>
-    <row r="69" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1">
+    <row r="69" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1">
       <c r="A69" s="38" t="str">
         <f>IF(LEFT(B69,2)="No",0,IF(LEFT(B69,7)="Partial",0.01,IF(LEFT(B69,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3259,7 +3259,7 @@
       </c>
       <c r="E69" s="25"/>
     </row>
-    <row r="70" spans="1:5" s="3" customFormat="1" ht="16" customHeight="1" thickBot="1">
+    <row r="70" spans="1:5" s="3" customFormat="1" ht="15.95" customHeight="1" thickBot="1">
       <c r="A70" s="39" t="str">
         <f>IF(LEFT(B70,2)="No",0,IF(LEFT(B70,7)="Partial",0.01,IF(LEFT(B70,4)="Full",0.02,"n/a")))</f>
         <v>n/a</v>
@@ -3459,9 +3459,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="89.6328125" customWidth="1"/>
+    <col min="1" max="1" width="89.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="24" thickBot="1">
@@ -3469,7 +3469,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="20" customFormat="1" ht="16" thickBot="1">
+    <row r="2" spans="1:1" s="20" customFormat="1" ht="16.5" thickBot="1">
       <c r="A2" s="21" t="str">
         <f>IF(LEN(A3) &gt; 1000,"",IF(LEN(A3) &gt; 500,"You need more post-mortem reflection.",IF(A3&gt;0,IF(A3="If you think you have accomplished one or more bonus goals that you are worried might be overlooked, mention those here.","How did the project go? What did you learn? What could you improve?","You need A LOT MORE post-mortem reflection."),"How did the project go? What did you learn? What could you improve?")))</f>
         <v>You need A LOT MORE post-mortem reflection.</v>
@@ -3493,15 +3493,15 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.6328125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.90625" style="28"/>
-    <col min="6" max="6" width="8.90625" style="29"/>
-    <col min="7" max="7" width="11.54296875" style="28" customWidth="1"/>
-    <col min="8" max="11" width="11.54296875" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="8.90625" style="2"/>
+    <col min="1" max="2" width="10.5703125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="28"/>
+    <col min="6" max="6" width="8.85546875" style="29"/>
+    <col min="7" max="7" width="11.5703125" style="28" customWidth="1"/>
+    <col min="8" max="11" width="11.5703125" style="29" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="24" thickBot="1">
@@ -3519,7 +3519,7 @@
       <c r="J1" s="61"/>
       <c r="K1" s="61"/>
     </row>
-    <row r="2" spans="1:11" ht="34.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:11" ht="34.35" customHeight="1" thickBot="1">
       <c r="A2" s="62" t="s">
         <v>78</v>
       </c>
@@ -3551,15 +3551,15 @@
       <selection activeCell="A2" sqref="A2:K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.6328125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.90625" style="28"/>
-    <col min="6" max="6" width="8.90625" style="29"/>
-    <col min="7" max="7" width="11.54296875" style="28" customWidth="1"/>
-    <col min="8" max="11" width="11.54296875" style="29" customWidth="1"/>
-    <col min="12" max="16384" width="8.90625" style="2"/>
+    <col min="1" max="2" width="10.5703125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="28"/>
+    <col min="6" max="6" width="8.85546875" style="29"/>
+    <col min="7" max="7" width="11.5703125" style="28" customWidth="1"/>
+    <col min="8" max="11" width="11.5703125" style="29" customWidth="1"/>
+    <col min="12" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="24" thickBot="1">
@@ -3577,7 +3577,7 @@
       <c r="J1" s="61"/>
       <c r="K1" s="61"/>
     </row>
-    <row r="2" spans="1:11" ht="34.25" customHeight="1" thickBot="1">
+    <row r="2" spans="1:11" ht="34.35" customHeight="1" thickBot="1">
       <c r="A2" s="62" t="s">
         <v>79</v>
       </c>
@@ -3607,10 +3607,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" customWidth="1"/>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -3620,7 +3620,7 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+    <row r="2" spans="1:3" ht="16.5" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -3629,10 +3629,10 @@
         <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="15"/>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -3641,10 +3641,10 @@
         <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1">
+    <row r="5" spans="1:3" ht="16.5" thickBot="1">
       <c r="A5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
@@ -3653,11 +3653,11 @@
         <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1">
       <c r="A7" s="15"/>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -3666,11 +3666,11 @@
         <v>&lt;-- Rough total session length in minutes.</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1">
       <c r="A9" s="15"/>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -3683,7 +3683,7 @@
       <c r="B11" s="66"/>
       <c r="C11" s="67"/>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
@@ -3697,7 +3697,7 @@
       <c r="B13" s="66"/>
       <c r="C13" s="67"/>
     </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
@@ -3711,7 +3711,7 @@
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
@@ -3725,7 +3725,7 @@
       <c r="B17" s="66"/>
       <c r="C17" s="67"/>
     </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
@@ -3734,12 +3734,12 @@
         <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A19" s="65"/>
       <c r="B19" s="66"/>
       <c r="C19" s="67"/>
     </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A21" s="68"/>
       <c r="B21" s="69"/>
       <c r="C21" s="70"/>
@@ -3777,10 +3777,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" customWidth="1"/>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -3790,7 +3790,7 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+    <row r="2" spans="1:3" ht="16.5" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -3799,10 +3799,10 @@
         <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="15"/>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -3811,10 +3811,10 @@
         <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1">
+    <row r="5" spans="1:3" ht="16.5" thickBot="1">
       <c r="A5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
@@ -3823,11 +3823,11 @@
         <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1">
       <c r="A7" s="15"/>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -3836,11 +3836,11 @@
         <v>&lt;-- Rough total session length in minutes.</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1">
       <c r="A9" s="15"/>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -3853,7 +3853,7 @@
       <c r="B11" s="66"/>
       <c r="C11" s="67"/>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
@@ -3867,7 +3867,7 @@
       <c r="B13" s="66"/>
       <c r="C13" s="67"/>
     </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
@@ -3881,7 +3881,7 @@
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
@@ -3895,7 +3895,7 @@
       <c r="B17" s="66"/>
       <c r="C17" s="67"/>
     </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
@@ -3904,12 +3904,12 @@
         <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A19" s="65"/>
       <c r="B19" s="66"/>
       <c r="C19" s="67"/>
     </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -3918,7 +3918,7 @@
         <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A21" s="68"/>
       <c r="B21" s="69"/>
       <c r="C21" s="70"/>
@@ -3947,10 +3947,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" customWidth="1"/>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -3960,7 +3960,7 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+    <row r="2" spans="1:3" ht="16.5" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -3969,10 +3969,10 @@
         <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="15"/>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -3981,10 +3981,10 @@
         <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1">
+    <row r="5" spans="1:3" ht="16.5" thickBot="1">
       <c r="A5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
@@ -3993,11 +3993,11 @@
         <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1">
       <c r="A7" s="15"/>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -4006,11 +4006,11 @@
         <v>&lt;-- Rough total session length in minutes.</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1">
       <c r="A9" s="15"/>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -4023,7 +4023,7 @@
       <c r="B11" s="66"/>
       <c r="C11" s="67"/>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
@@ -4037,7 +4037,7 @@
       <c r="B13" s="66"/>
       <c r="C13" s="67"/>
     </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
@@ -4051,7 +4051,7 @@
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
@@ -4065,7 +4065,7 @@
       <c r="B17" s="66"/>
       <c r="C17" s="67"/>
     </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
@@ -4074,12 +4074,12 @@
         <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A19" s="65"/>
       <c r="B19" s="66"/>
       <c r="C19" s="67"/>
     </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -4088,7 +4088,7 @@
         <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A21" s="68"/>
       <c r="B21" s="69"/>
       <c r="C21" s="70"/>
@@ -4117,10 +4117,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" customWidth="1"/>
-    <col min="2" max="2" width="37.54296875" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" thickBot="1">
@@ -4130,7 +4130,7 @@
       <c r="B1" s="11"/>
       <c r="C1" s="11"/>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1">
+    <row r="2" spans="1:3" ht="16.5" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -4139,10 +4139,10 @@
         <v>&lt;-- What lab goals had already been met at the time of this test (roughly)?</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1">
+    <row r="3" spans="1:3" ht="16.5" thickBot="1">
       <c r="A3" s="15"/>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1">
+    <row r="4" spans="1:3" ht="16.5" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
@@ -4151,10 +4151,10 @@
         <v>&lt;-- What date did the playtest occur (time of day not needed)?</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1">
+    <row r="5" spans="1:3" ht="16.5" thickBot="1">
       <c r="A5" s="16"/>
     </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1">
+    <row r="6" spans="1:3" ht="16.5" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
@@ -4163,11 +4163,11 @@
         <v>&lt;-- Where did the playtest occur (room name, 'tester's apartment', etc.)?</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1">
+    <row r="7" spans="1:3" ht="16.5" thickBot="1">
       <c r="A7" s="15"/>
       <c r="B7" s="9"/>
     </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1">
+    <row r="8" spans="1:3" ht="16.5" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -4176,11 +4176,11 @@
         <v>&lt;-- Rough total session length in minutes.</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1">
+    <row r="9" spans="1:3" ht="16.5" thickBot="1">
       <c r="A9" s="15"/>
       <c r="B9" s="9"/>
     </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1">
+    <row r="10" spans="1:3" ht="16.5" thickBot="1">
       <c r="A10" s="13" t="s">
         <v>7</v>
       </c>
@@ -4193,7 +4193,7 @@
       <c r="B11" s="66"/>
       <c r="C11" s="67"/>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1">
+    <row r="12" spans="1:3" ht="16.5" thickBot="1">
       <c r="A12" s="14" t="s">
         <v>2</v>
       </c>
@@ -4207,7 +4207,7 @@
       <c r="B13" s="66"/>
       <c r="C13" s="67"/>
     </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1">
+    <row r="14" spans="1:3" ht="16.5" thickBot="1">
       <c r="A14" s="13" t="s">
         <v>3</v>
       </c>
@@ -4221,7 +4221,7 @@
       <c r="B15" s="66"/>
       <c r="C15" s="67"/>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1">
+    <row r="16" spans="1:3" ht="16.5" thickBot="1">
       <c r="A16" s="13" t="s">
         <v>9</v>
       </c>
@@ -4235,7 +4235,7 @@
       <c r="B17" s="66"/>
       <c r="C17" s="67"/>
     </row>
-    <row r="18" spans="1:3" ht="16" thickBot="1">
+    <row r="18" spans="1:3" ht="16.5" thickBot="1">
       <c r="A18" s="13" t="s">
         <v>10</v>
       </c>
@@ -4244,12 +4244,12 @@
         <v>&lt;-- Explain observations, data, or patterns from the playtest. What did you learn or have confirmed?</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="19" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A19" s="65"/>
       <c r="B19" s="66"/>
       <c r="C19" s="67"/>
     </row>
-    <row r="20" spans="1:3" ht="16" thickBot="1">
+    <row r="20" spans="1:3" ht="16.5" thickBot="1">
       <c r="A20" s="13" t="s">
         <v>11</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>&lt;-- What changes would you recommend be made, and what do you think needs further research?</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="110.15" customHeight="1" thickBot="1">
+    <row r="21" spans="1:3" ht="110.1" customHeight="1" thickBot="1">
       <c r="A21" s="68"/>
       <c r="B21" s="69"/>
       <c r="C21" s="70"/>

</xml_diff>